<commit_message>
Corrección en Captura y Edición de Conceptos, sección Niveles de Autorizadores
</commit_message>
<xml_diff>
--- a/Documentos/Reportes de Pruebas/Estatus NM Pendientes v4.xlsx
+++ b/Documentos/Reportes de Pruebas/Estatus NM Pendientes v4.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="58">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">Responsable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha estimada</t>
   </si>
   <si>
     <t xml:space="preserve">Estatus</t>
@@ -74,7 +77,7 @@
     <t xml:space="preserve">Inmediato en la operación de la app.</t>
   </si>
   <si>
-    <t xml:space="preserve">Jesus   mie-18</t>
+    <t xml:space="preserve">Jesús</t>
   </si>
   <si>
     <t xml:space="preserve">En Desarrollo/ Indispensable</t>
@@ -92,9 +95,6 @@
     <t xml:space="preserve">Informativo para usuario Administrador</t>
   </si>
   <si>
-    <t xml:space="preserve">Javier lun 23</t>
-  </si>
-  <si>
     <t xml:space="preserve">En Desarrollo/Indispensable</t>
   </si>
   <si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t xml:space="preserve">Realizar pruebas de autorizaciones automáticas por montos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jesus jue-19</t>
   </si>
   <si>
     <t xml:space="preserve">Pospuesto/ indispensable</t>
@@ -141,16 +138,10 @@
     <t xml:space="preserve">Al capturarse una solicitud, debe revisarse que se actualicen los conceptos que indique la configuración de Autorización Automática.</t>
   </si>
   <si>
-    <t xml:space="preserve">jesus lun-23</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pantalla de Consulta para Autorizantes</t>
   </si>
   <si>
     <t xml:space="preserve">Los Autorizantes podrán acceder a consulta de Autorizaciones independiente de Mis Autorizaciones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jesus mar-24</t>
   </si>
   <si>
     <t xml:space="preserve">Indispensable</t>
@@ -165,9 +156,6 @@
   <si>
     <t xml:space="preserve">Al capturarse una solicitud, el usuario no tiene la opción de capturar la nómina a la que se aplicará, por una simplificación solicitada por Luis en la pantalla de Captura Rápida.
 Esta funcionalidad requiere realizar pruebas de Captura de Solicitudes para Períodos Futuros.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jesus vie-27</t>
   </si>
   <si>
     <t xml:space="preserve">Pospuesta/Indispensable</t>
@@ -236,10 +224,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$$-80A]#,##0.00;[RED]\-[$$-80A]#,##0.00"/>
     <numFmt numFmtId="166" formatCode="[$-80A]General"/>
+    <numFmt numFmtId="167" formatCode="[$-80A]D&quot; de &quot;MMM&quot; de &quot;YYYY"/>
+    <numFmt numFmtId="168" formatCode="D&quot; de &quot;MMM&quot; de &quot;YYYY"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -445,13 +435,13 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -459,17 +449,25 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -482,11 +480,19 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="23" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -511,27 +517,35 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -621,385 +635,401 @@
   </sheetPr>
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="4.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="57.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="31.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="10.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="13.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="37.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="69.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="31.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="13.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="19.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="14.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="2" width="21.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="33.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="10" style="2" width="21.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="10.5"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="43.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I1" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="G2" s="7"/>
+      <c r="H2" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I2" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="D3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="9" t="s">
+      <c r="F3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="G3" s="11" t="n">
+        <v>43817</v>
+      </c>
+      <c r="H3" s="12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="41.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I3" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="B4" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="D4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="9" t="s">
+      <c r="F4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="11" t="n">
+        <v>43822</v>
+      </c>
+      <c r="H4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="B5" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="C5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="8" t="n">
+      <c r="D5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="F5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="14" t="n">
+        <v>43818</v>
+      </c>
+      <c r="H5" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="I5" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="B6" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="8" t="s">
+      <c r="D6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="10" t="n">
         <v>16</v>
       </c>
-      <c r="F6" s="8" t="n">
-        <v>16</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="11" t="s">
+      <c r="F6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="14" t="n">
+        <v>43822</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
+      <c r="B7" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="C7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="11" t="n">
+        <v>43823</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="8" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
+      <c r="B8" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="2" t="n">
-        <v>16</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="82.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="9" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
+      <c r="B9" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="C9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="2" t="n">
+        <v>41</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="2" t="n">
         <v>40</v>
       </c>
+      <c r="G9" s="11"/>
       <c r="H9" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="2" t="n">
+      <c r="B10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="H10" s="13" t="s">
-        <v>37</v>
+      <c r="G10" s="11"/>
+      <c r="H10" s="17" t="s">
+        <v>34</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="82.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="B11" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="C11" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="14"/>
-      <c r="H11" s="11" t="s">
-        <v>51</v>
+        <v>46</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="18"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="15" t="s">
+        <v>47</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="41.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
+      <c r="B12" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="C12" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="I12" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="18"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="I12" s="19" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="27.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
+      <c r="B13" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="C13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="18" t="n">
+        <v>12</v>
+      </c>
+      <c r="G13" s="11"/>
+      <c r="H13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="20"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="20"/>
+      <c r="C15" s="17"/>
+      <c r="H15" s="17"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="21"/>
+      <c r="B16" s="22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="23"/>
+      <c r="B17" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="25"/>
+      <c r="B18" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="26"/>
+      <c r="B19" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="2" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="27"/>
+      <c r="B20" s="28" t="s">
         <v>57</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="14" t="n">
-        <v>12</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="D15" s="13"/>
-      <c r="H15" s="13"/>
-    </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="19"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="22" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>